<commit_message>
admin page not complete
</commit_message>
<xml_diff>
--- a/Survey/통합 문서2.xlsx
+++ b/Survey/통합 문서2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\StaisfactionSurvey\Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61520A06-8E99-4906-9A2D-3F4ACB91251B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB65A34-C828-411D-A043-9182B7547A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17700" yWindow="3195" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,15 @@
     <sheet name="설문지 관리" sheetId="6" r:id="rId6"/>
     <sheet name="그룹항목" sheetId="9" r:id="rId7"/>
     <sheet name="항목" sheetId="7" r:id="rId8"/>
-    <sheet name="사용자응답" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
+    <sheet name="사용자응답" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="193">
   <si>
     <t>Table 정의서</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -166,10 +167,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>adm_name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>관리 권한</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -306,10 +303,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>성명</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>stu_name</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -674,10 +667,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Satisfaction Survey</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -781,6 +770,54 @@
   </si>
   <si>
     <t>항목 항목내용</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(3)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>xy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cde</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>단방향 암호화</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>adm_Name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 등록페이지</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -939,7 +976,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -963,6 +1000,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1337,62 +1377,62 @@
   <dimension ref="A4:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="A6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1406,12 +1446,204 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F1C121-4328-4C25-8B9A-93EC9448EDAD}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="9" max="9" width="25.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1454,7 +1686,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1478,6 +1710,64 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1487,51 +1777,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="9" max="9" width="36.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1565,7 +1856,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>23</v>
@@ -1575,7 +1866,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1592,7 +1883,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="4">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
@@ -1601,7 +1892,9 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1615,7 +1908,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1623,27 +1916,15 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
@@ -1651,68 +1932,91 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1722,6 +2026,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1730,7 +2035,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="A1:K28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1743,123 +2048,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C4" s="4">
         <v>9</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C5" s="4">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4">
         <v>20</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1868,40 +2173,40 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4">
         <v>50</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1910,17 +2215,17 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4">
         <v>50</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -1929,17 +2234,17 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4">
         <v>15</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1948,17 +2253,17 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4">
         <v>30</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1967,17 +2272,17 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1986,17 +2291,17 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="4">
         <v>100</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2005,17 +2310,17 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="4">
         <v>100</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -2024,63 +2329,63 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4">
         <v>6</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="4">
         <v>3</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2089,40 +2394,40 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4">
         <v>20</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4">
         <v>10</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2131,17 +2436,17 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4">
         <v>20</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2150,17 +2455,17 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="4">
         <v>255</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2180,15 +2485,15 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2197,44 +2502,44 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="4">
         <v>20</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2252,7 +2557,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="A2:L23"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2263,211 +2568,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="A1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+        <v>114</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="4">
         <v>5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4">
         <v>82</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4">
         <v>20</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4">
         <v>3</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -2509,15 +2814,15 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -2526,80 +2831,80 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C16" s="4">
         <v>20</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="A20" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2617,7 +2922,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="A1:J21"/>
+      <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2629,37 +2934,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2693,15 +2998,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2710,10 +3015,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2725,10 +3030,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2751,15 +3056,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -2768,7 +3073,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -2778,18 +3083,18 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>23</v>
@@ -2799,13 +3104,13 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2835,37 +3140,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2899,15 +3204,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2916,10 +3221,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2931,10 +3236,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2957,15 +3262,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -2974,7 +3279,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -2984,18 +3289,18 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>23</v>
@@ -3005,13 +3310,13 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3026,10 +3331,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDC4CBE-5ECC-4D63-B2D5-38B210E9EEEE}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3041,37 +3346,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3105,15 +3410,15 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3122,7 +3427,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3135,7 +3440,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3145,12 +3450,12 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3163,15 +3468,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -3180,7 +3485,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -3190,18 +3495,18 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>23</v>
@@ -3211,13 +3516,18 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3232,191 +3542,89 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F1C121-4328-4C25-8B9A-93EC9448EDAD}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9215610C-E5B9-481F-A3BA-B506CCA61EF7}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C12" sqref="C12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.125" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="9" max="9" width="25.25" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="E1" s="15" t="s">
+        <v>163</v>
+      </c>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="4">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="E3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:G2"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>